<commit_message>
Préparation publivation release 2.0.0-ballot (#342)
* Prepa release 200-ballot

* correctif pour publication

* Update sushi-config.yaml

* Update publication-request.json 294e12483dad8d756740d6d95e8107a06ea5f973
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-tddui-encounter-identifier.xlsx
+++ b/main/ig/CodeSystem-tddui-encounter-identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>2.0.0-ballot</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-31T15:04:06+00:00</t>
+    <t>2025-07-31T17:00:40+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Préparation de la publication de l'IG version 2.0.0 (#370)
* Preparation release 200

* preparation release 200 0d694ec3b22fd71e8e4b8d595504e8a461026a95
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-tddui-encounter-identifier.xlsx
+++ b/main/ig/CodeSystem-tddui-encounter-identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-ballot</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-19T12:04:16+00:00</t>
+    <t>2025-09-24T12:27:45+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>